<commit_message>
cleaning code more, updating suppl table 5 so no age standards on age groups
</commit_message>
<xml_diff>
--- a/tables/alt_education_table.xlsx
+++ b/tables/alt_education_table.xlsx
@@ -558,57 +558,57 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.19</t>
+          <t>0.21</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.38</t>
+          <t>0.42</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.28</t>
+          <t>0.3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.43</t>
+          <t>0.45</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.53</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.47</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0.48</t>
+          <t>0.53</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>0.53</t>
+          <t>0.56</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.58</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.55</t>
+          <t>0.59</t>
         </is>
       </c>
     </row>
@@ -875,57 +875,57 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>0.26</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.45</t>
+          <t>0.49</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.35</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0.42</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.57</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
           <t>0.47</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>0.39</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>0.53</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>0.45</t>
-        </is>
-      </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>0.61</t>
+          <t>0.65</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.59</t>
+          <t>0.62</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.56</t>
+          <t>0.6</t>
         </is>
       </c>
     </row>

</xml_diff>